<commit_message>
Improved the volatility point for better rating.
</commit_message>
<xml_diff>
--- a/portfolio_rankings.xlsx
+++ b/portfolio_rankings.xlsx
@@ -599,7 +599,7 @@
         <v>65</v>
       </c>
       <c r="L2" t="n">
-        <v>35.45860667649082</v>
+        <v>35.45860667648925</v>
       </c>
       <c r="M2" t="n">
         <v>45</v>
@@ -614,11 +614,11 @@
         <v>25</v>
       </c>
       <c r="Q2" t="n">
-        <v>30.38357016651501</v>
+        <v>30.38357733960528</v>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>Fetched fundamental data for NXPI; Calculated technical metrics for NXPI; Promoter Holding: 50.0% -&gt; Score: 100; Institutional Holding: 10.0% -&gt; Score: 40.0; Debt-to-Equity Ratio: 116.945 -&gt; Score: 0; Return on Equity: 27.49% -&gt; Score: 100; Profit Growth YoY: 15.0% -&gt; Score: 75.0; Profit CAGR 5Y: 10.0% -&gt; Score: 50.0; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667649082; NIFTY200DMARSIVolume: Price &lt;= 200-Day DMA (+0); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &lt;= 50 (+10); NIFTY200DMARSIVolume: Total Score: 45; 200-Day DMA: Below -&gt; Score: 0; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.383570166515007; Volatility: 0.50 -&gt; Penalty: 0.50; Final Rating: 22.45; Promoter Holding: 50.0% -&gt; Score: 100; Institutional Holding: 10.0% -&gt; Score: 40.0; Debt-to-Equity Ratio: 116.945 -&gt; Score: 0; Return on Equity: 27.49% -&gt; Score: 100; Profit Growth YoY: 15.0% -&gt; Score: 75.0; Profit CAGR 5Y: 10.0% -&gt; Score: 50.0; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667649082; NIFTY200DMARSIVolume: Price &lt;= 200-Day DMA (+0); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &lt;= 50 (+10); NIFTY200DMARSIVolume: Total Score: 45; 200-Day DMA: Below -&gt; Score: 0; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.383570166515007; Volatility: 0.50 -&gt; Penalty: 0.50; Final Rating: 22.45; Promoter Holding: 50.0% -&gt; Score: 100; Institutional Holding: 10.0% -&gt; Score: 40.0; Debt-to-Equity Ratio: 116.945 -&gt; Score: 0; Return on Equity: 27.49% -&gt; Score: 100; Profit Growth YoY: 15.0% -&gt; Score: 75.0; Profit CAGR 5Y: 10.0% -&gt; Score: 50.0; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667649082; NIFTY200DMARSIVolume: Price &lt;= 200-Day DMA (+0); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &lt;= 50 (+10); NIFTY200DMARSIVolume: Total Score: 45; 200-Day DMA: Below -&gt; Score: 0; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.383570166515007; Volatility: 0.50 -&gt; Penalty: 0.50; Final Rating: 22.45; Promoter Holding: 50.0% -&gt; Score: 100; Institutional Holding: 10.0% -&gt; Score: 40.0; Debt-to-Equity Ratio: 116.945 -&gt; Score: 0; Return on Equity: 27.49% -&gt; Score: 100; Profit Growth YoY: 15.0% -&gt; Score: 75.0; Profit CAGR 5Y: 10.0% -&gt; Score: 50.0; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667649082; NIFTY200DMARSIVolume: Price &lt;= 200-Day DMA (+0); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &lt;= 50 (+10); NIFTY200DMARSIVolume: Total Score: 45; 200-Day DMA: Below -&gt; Score: 0; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.383570166515007; Volatility: 0.50 -&gt; Penalty: 0.50; Final Rating: 22.45; Promoter Holding: 50.0% -&gt; Score: 100; Institutional Holding: 10.0% -&gt; Score: 40.0; Debt-to-Equity Ratio: 116.945 -&gt; Score: 0; Return on Equity: 27.49% -&gt; Score: 100; Profit Growth YoY: 15.0% -&gt; Score: 75.0; Profit CAGR 5Y: 10.0% -&gt; Score: 50.0; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667649082; NIFTY200DMARSIVolume: Price &lt;= 200-Day DMA (+0); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &lt;= 50 (+10); NIFTY200DMARSIVolume: Total Score: 45; 200-Day DMA: Below -&gt; Score: 0; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.383570166515007; Volatility: 0.50 -&gt; Penalty: 0.50; Final Rating: 22.45; Promoter Holding: 50.0% -&gt; Score: 100; Institutional Holding: 10.0% -&gt; Score: 40.0; Debt-to-Equity Ratio: 116.945 -&gt; Score: 0; Return on Equity: 27.49% -&gt; Score: 100; Profit Growth YoY: 15.0% -&gt; Score: 75.0; Profit CAGR 5Y: 10.0% -&gt; Score: 50.0; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667649082; NIFTY200DMARSIVolume: Price &lt;= 200-Day DMA (+0); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &lt;= 50 (+10); NIFTY200DMARSIVolume: Total Score: 45; 200-Day DMA: Below -&gt; Score: 0; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.383570166515007; Volatility: 0.50 -&gt; Penalty: 0.50; Final Rating: 22.45; Promoter Holding: 50.0% -&gt; Score: 100; Institutional Holding: 10.0% -&gt; Score: 40.0; Debt-to-Equity Ratio: 116.945 -&gt; Score: 0; Return on Equity: 27.49% -&gt; Score: 100; Profit Growth YoY: 15.0% -&gt; Score: 75.0; Profit CAGR 5Y: 10.0% -&gt; Score: 50.0; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667649082; NIFTY200DMARSIVolume: Price &lt;= 200-Day DMA (+0); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &lt;= 50 (+10); NIFTY200DMARSIVolume: Total Score: 45; 200-Day DMA: Below -&gt; Score: 0; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.383570166515007; Volatility: 0.50 -&gt; Penalty: 0.50; Final Rating: 22.45; Promoter Holding: 50.0% -&gt; Score: 100; Institutional Holding: 10.0% -&gt; Score: 40.0; Debt-to-Equity Ratio: 116.945 -&gt; Score: 0; Return on Equity: 27.49% -&gt; Score: 100; Profit Growth YoY: 15.0% -&gt; Score: 75.0; Profit CAGR 5Y: 10.0% -&gt; Score: 50.0; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667649082; NIFTY200DMARSIVolume: Price &lt;= 200-Day DMA (+0); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &lt;= 50 (+10); NIFTY200DMARSIVolume: Total Score: 45; 200-Day DMA: Below -&gt; Score: 0; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.383570166515007; Volatility: 0.50 -&gt; Penalty: 0.50; Final Rating: 22.45</t>
+          <t>Fetched fundamental data for NXPI; Calculated technical metrics for NXPI; Promoter Holding: 50.0% -&gt; Score: 100; Institutional Holding: 10.0% -&gt; Score: 40.0; Debt-to-Equity Ratio: 116.945 -&gt; Score: 0; Return on Equity: 27.49% -&gt; Score: 100; Profit Growth YoY: 15.0% -&gt; Score: 75.0; Profit CAGR 5Y: 10.0% -&gt; Score: 50.0; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667648925; NIFTY200DMARSIVolume: Price &lt;= 200-Day DMA (+0); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &lt;= 50 (+10); NIFTY200DMARSIVolume: Total Score: 45; 200-Day DMA: Below -&gt; Score: 0; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.38357733960528; Volatility: 0.50 -&gt; Penalty: 0.50; Final Rating: 22.45; Promoter Holding: 50.0% -&gt; Score: 100; Institutional Holding: 10.0% -&gt; Score: 40.0; Debt-to-Equity Ratio: 116.945 -&gt; Score: 0; Return on Equity: 27.49% -&gt; Score: 100; Profit Growth YoY: 15.0% -&gt; Score: 75.0; Profit CAGR 5Y: 10.0% -&gt; Score: 50.0; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667648925; NIFTY200DMARSIVolume: Price &lt;= 200-Day DMA (+0); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &lt;= 50 (+10); NIFTY200DMARSIVolume: Total Score: 45; 200-Day DMA: Below -&gt; Score: 0; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.38357733960528; Volatility: 0.50 -&gt; Penalty: 0.50; Final Rating: 22.45; Promoter Holding: 50.0% -&gt; Score: 100; Institutional Holding: 10.0% -&gt; Score: 40.0; Debt-to-Equity Ratio: 116.945 -&gt; Score: 0; Return on Equity: 27.49% -&gt; Score: 100; Profit Growth YoY: 15.0% -&gt; Score: 75.0; Profit CAGR 5Y: 10.0% -&gt; Score: 50.0; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667648925; NIFTY200DMARSIVolume: Price &lt;= 200-Day DMA (+0); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &lt;= 50 (+10); NIFTY200DMARSIVolume: Total Score: 45; 200-Day DMA: Below -&gt; Score: 0; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.38357733960528; Volatility: 0.50 -&gt; Penalty: 0.50; Final Rating: 22.45; Promoter Holding: 50.0% -&gt; Score: 100; Institutional Holding: 10.0% -&gt; Score: 40.0; Debt-to-Equity Ratio: 116.945 -&gt; Score: 0; Return on Equity: 27.49% -&gt; Score: 100; Profit Growth YoY: 15.0% -&gt; Score: 75.0; Profit CAGR 5Y: 10.0% -&gt; Score: 50.0; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667648925; NIFTY200DMARSIVolume: Price &lt;= 200-Day DMA (+0); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &lt;= 50 (+10); NIFTY200DMARSIVolume: Total Score: 45; 200-Day DMA: Below -&gt; Score: 0; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.38357733960528; Volatility: 0.50 -&gt; Penalty: 0.50; Final Rating: 22.45; Promoter Holding: 50.0% -&gt; Score: 100; Institutional Holding: 10.0% -&gt; Score: 40.0; Debt-to-Equity Ratio: 116.945 -&gt; Score: 0; Return on Equity: 27.49% -&gt; Score: 100; Profit Growth YoY: 15.0% -&gt; Score: 75.0; Profit CAGR 5Y: 10.0% -&gt; Score: 50.0; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667648925; NIFTY200DMARSIVolume: Price &lt;= 200-Day DMA (+0); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &lt;= 50 (+10); NIFTY200DMARSIVolume: Total Score: 45; 200-Day DMA: Below -&gt; Score: 0; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.38357733960528; Volatility: 0.50 -&gt; Penalty: 0.50; Final Rating: 22.45; Promoter Holding: 50.0% -&gt; Score: 100; Institutional Holding: 10.0% -&gt; Score: 40.0; Debt-to-Equity Ratio: 116.945 -&gt; Score: 0; Return on Equity: 27.49% -&gt; Score: 100; Profit Growth YoY: 15.0% -&gt; Score: 75.0; Profit CAGR 5Y: 10.0% -&gt; Score: 50.0; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667648925; NIFTY200DMARSIVolume: Price &lt;= 200-Day DMA (+0); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &lt;= 50 (+10); NIFTY200DMARSIVolume: Total Score: 45; 200-Day DMA: Below -&gt; Score: 0; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.38357733960528; Volatility: 0.50 -&gt; Penalty: 0.50; Final Rating: 22.45; Promoter Holding: 50.0% -&gt; Score: 100; Institutional Holding: 10.0% -&gt; Score: 40.0; Debt-to-Equity Ratio: 116.945 -&gt; Score: 0; Return on Equity: 27.49% -&gt; Score: 100; Profit Growth YoY: 15.0% -&gt; Score: 75.0; Profit CAGR 5Y: 10.0% -&gt; Score: 50.0; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667648925; NIFTY200DMARSIVolume: Price &lt;= 200-Day DMA (+0); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &lt;= 50 (+10); NIFTY200DMARSIVolume: Total Score: 45; 200-Day DMA: Below -&gt; Score: 0; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.38357733960528; Volatility: 0.50 -&gt; Penalty: 0.50; Final Rating: 22.45; Promoter Holding: 50.0% -&gt; Score: 100; Institutional Holding: 10.0% -&gt; Score: 40.0; Debt-to-Equity Ratio: 116.945 -&gt; Score: 0; Return on Equity: 27.49% -&gt; Score: 100; Profit Growth YoY: 15.0% -&gt; Score: 75.0; Profit CAGR 5Y: 10.0% -&gt; Score: 50.0; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667648925; NIFTY200DMARSIVolume: Price &lt;= 200-Day DMA (+0); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &lt;= 50 (+10); NIFTY200DMARSIVolume: Total Score: 45; 200-Day DMA: Below -&gt; Score: 0; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.38357733960528; Volatility: 0.50 -&gt; Penalty: 0.50; Final Rating: 22.45</t>
         </is>
       </c>
     </row>
@@ -629,16 +629,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>23.69</v>
+        <v>24.3</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>50.6% -&gt; 100</t>
+          <t>59.4% -&gt; 100</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>8.7% -&gt; 34.8</t>
+          <t>3.0% -&gt; 12.0</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -653,12 +653,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>38.5% -&gt; 100</t>
+          <t>34.0% -&gt; 100</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>11.5% -&gt; 57.5</t>
+          <t>85.0% -&gt; 100</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -694,7 +694,7 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>Fetched fundamental data for AXISCADES.NS; Calculated technical metrics for AXISCADES.NS; Promoter Holding: 50.6% -&gt; Score: 100; Institutional Holding: 8.7% -&gt; Score: 34.8; Debt-to-Equity Ratio: 41.604 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 38.5% -&gt; Score: 100; Profit CAGR 5Y: 11.5% -&gt; Score: 57.5; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=51.32, MACD=Negative -&gt; Score: 25.329054366958594; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.58 -&gt; Penalty: 0.42; Final Rating: 23.69; Promoter Holding: 50.6% -&gt; Score: 100; Institutional Holding: 8.7% -&gt; Score: 34.8; Debt-to-Equity Ratio: 41.604 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 38.5% -&gt; Score: 100; Profit CAGR 5Y: 11.5% -&gt; Score: 57.5; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=51.32, MACD=Negative -&gt; Score: 25.329054366958594; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.58 -&gt; Penalty: 0.42; Final Rating: 23.69; Promoter Holding: 50.6% -&gt; Score: 100; Institutional Holding: 8.7% -&gt; Score: 34.8; Debt-to-Equity Ratio: 41.604 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 38.5% -&gt; Score: 100; Profit CAGR 5Y: 11.5% -&gt; Score: 57.5; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=51.32, MACD=Negative -&gt; Score: 25.329054366958594; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.58 -&gt; Penalty: 0.42; Final Rating: 23.69; Promoter Holding: 50.6% -&gt; Score: 100; Institutional Holding: 8.7% -&gt; Score: 34.8; Debt-to-Equity Ratio: 41.604 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 38.5% -&gt; Score: 100; Profit CAGR 5Y: 11.5% -&gt; Score: 57.5; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=51.32, MACD=Negative -&gt; Score: 25.329054366958594; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.58 -&gt; Penalty: 0.42; Final Rating: 23.69; Promoter Holding: 50.6% -&gt; Score: 100; Institutional Holding: 8.7% -&gt; Score: 34.8; Debt-to-Equity Ratio: 41.604 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 38.5% -&gt; Score: 100; Profit CAGR 5Y: 11.5% -&gt; Score: 57.5; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=51.32, MACD=Negative -&gt; Score: 25.329054366958594; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.58 -&gt; Penalty: 0.42; Final Rating: 23.69; Promoter Holding: 50.6% -&gt; Score: 100; Institutional Holding: 8.7% -&gt; Score: 34.8; Debt-to-Equity Ratio: 41.604 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 38.5% -&gt; Score: 100; Profit CAGR 5Y: 11.5% -&gt; Score: 57.5; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=51.32, MACD=Negative -&gt; Score: 25.329054366958594; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.58 -&gt; Penalty: 0.42; Final Rating: 23.69; Promoter Holding: 50.6% -&gt; Score: 100; Institutional Holding: 8.7% -&gt; Score: 34.8; Debt-to-Equity Ratio: 41.604 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 38.5% -&gt; Score: 100; Profit CAGR 5Y: 11.5% -&gt; Score: 57.5; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=51.32, MACD=Negative -&gt; Score: 25.329054366958594; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.58 -&gt; Penalty: 0.42; Final Rating: 23.69; Promoter Holding: 50.6% -&gt; Score: 100; Institutional Holding: 8.7% -&gt; Score: 34.8; Debt-to-Equity Ratio: 41.604 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 38.5% -&gt; Score: 100; Profit CAGR 5Y: 11.5% -&gt; Score: 57.5; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=51.32, MACD=Negative -&gt; Score: 25.329054366958594; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.58 -&gt; Penalty: 0.42; Final Rating: 23.69</t>
+          <t>Fetched fundamental data for AXISCADES.NS; Calculated technical metrics for AXISCADES.NS; Promoter Holding: 59.4% -&gt; Score: 100; Institutional Holding: 3.0% -&gt; Score: 12.0; Debt-to-Equity Ratio: 41.604 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 34.0% -&gt; Score: 100; Profit CAGR 5Y: 85.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=51.32, MACD=Negative -&gt; Score: 25.329054366958594; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.58 -&gt; Penalty: 0.42; Final Rating: 24.3; Promoter Holding: 59.4% -&gt; Score: 100; Institutional Holding: 3.0% -&gt; Score: 12.0; Debt-to-Equity Ratio: 41.604 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 34.0% -&gt; Score: 100; Profit CAGR 5Y: 85.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=51.32, MACD=Negative -&gt; Score: 25.329054366958594; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.58 -&gt; Penalty: 0.42; Final Rating: 24.3; Promoter Holding: 59.4% -&gt; Score: 100; Institutional Holding: 3.0% -&gt; Score: 12.0; Debt-to-Equity Ratio: 41.604 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 34.0% -&gt; Score: 100; Profit CAGR 5Y: 85.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=51.32, MACD=Negative -&gt; Score: 25.329054366958594; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.58 -&gt; Penalty: 0.42; Final Rating: 24.3; Promoter Holding: 59.4% -&gt; Score: 100; Institutional Holding: 3.0% -&gt; Score: 12.0; Debt-to-Equity Ratio: 41.604 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 34.0% -&gt; Score: 100; Profit CAGR 5Y: 85.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=51.32, MACD=Negative -&gt; Score: 25.329054366958594; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.58 -&gt; Penalty: 0.42; Final Rating: 24.3; Promoter Holding: 59.4% -&gt; Score: 100; Institutional Holding: 3.0% -&gt; Score: 12.0; Debt-to-Equity Ratio: 41.604 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 34.0% -&gt; Score: 100; Profit CAGR 5Y: 85.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=51.32, MACD=Negative -&gt; Score: 25.329054366958594; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.58 -&gt; Penalty: 0.42; Final Rating: 24.3; Promoter Holding: 59.4% -&gt; Score: 100; Institutional Holding: 3.0% -&gt; Score: 12.0; Debt-to-Equity Ratio: 41.604 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 34.0% -&gt; Score: 100; Profit CAGR 5Y: 85.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=51.32, MACD=Negative -&gt; Score: 25.329054366958594; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.58 -&gt; Penalty: 0.42; Final Rating: 24.3; Promoter Holding: 59.4% -&gt; Score: 100; Institutional Holding: 3.0% -&gt; Score: 12.0; Debt-to-Equity Ratio: 41.604 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 34.0% -&gt; Score: 100; Profit CAGR 5Y: 85.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=51.32, MACD=Negative -&gt; Score: 25.329054366958594; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.58 -&gt; Penalty: 0.42; Final Rating: 24.3; Promoter Holding: 59.4% -&gt; Score: 100; Institutional Holding: 3.0% -&gt; Score: 12.0; Debt-to-Equity Ratio: 41.604 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 34.0% -&gt; Score: 100; Profit CAGR 5Y: 85.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=51.32, MACD=Negative -&gt; Score: 25.329054366958594; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.58 -&gt; Penalty: 0.42; Final Rating: 24.3</t>
         </is>
       </c>
     </row>
@@ -705,16 +705,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>27.07</v>
+        <v>29.09</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>60.0% -&gt; 100</t>
+          <t>61.0% -&gt; 100</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>10.0% -&gt; 40.0</t>
+          <t>39.0% -&gt; 100</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -729,12 +729,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>20.0% -&gt; 100</t>
+          <t>78.0% -&gt; 100</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>25.0% -&gt; 100</t>
+          <t>35.0% -&gt; 100</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -770,7 +770,7 @@
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>Fetched fundamental data for CARTRADE.NS; Calculated technical metrics for CARTRADE.NS; Promoter Holding: 60.0% -&gt; Score: 100; Institutional Holding: 10.0% -&gt; Score: 40.0; Debt-to-Equity Ratio: 5.514 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 20.0% -&gt; Score: 100; Profit CAGR 5Y: 25.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=48.71, MACD=Negative -&gt; Score: 24.677932862963523; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.54 -&gt; Penalty: 0.46; Final Rating: 27.07; Promoter Holding: 60.0% -&gt; Score: 100; Institutional Holding: 10.0% -&gt; Score: 40.0; Debt-to-Equity Ratio: 5.514 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 20.0% -&gt; Score: 100; Profit CAGR 5Y: 25.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=48.71, MACD=Negative -&gt; Score: 24.677932862963523; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.54 -&gt; Penalty: 0.46; Final Rating: 27.07; Promoter Holding: 60.0% -&gt; Score: 100; Institutional Holding: 10.0% -&gt; Score: 40.0; Debt-to-Equity Ratio: 5.514 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 20.0% -&gt; Score: 100; Profit CAGR 5Y: 25.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=48.71, MACD=Negative -&gt; Score: 24.677932862963523; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.54 -&gt; Penalty: 0.46; Final Rating: 27.07; Promoter Holding: 60.0% -&gt; Score: 100; Institutional Holding: 10.0% -&gt; Score: 40.0; Debt-to-Equity Ratio: 5.514 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 20.0% -&gt; Score: 100; Profit CAGR 5Y: 25.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=48.71, MACD=Negative -&gt; Score: 24.677932862963523; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.54 -&gt; Penalty: 0.46; Final Rating: 27.07; Promoter Holding: 60.0% -&gt; Score: 100; Institutional Holding: 10.0% -&gt; Score: 40.0; Debt-to-Equity Ratio: 5.514 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 20.0% -&gt; Score: 100; Profit CAGR 5Y: 25.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=48.71, MACD=Negative -&gt; Score: 24.677932862963523; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.54 -&gt; Penalty: 0.46; Final Rating: 27.07; Promoter Holding: 60.0% -&gt; Score: 100; Institutional Holding: 10.0% -&gt; Score: 40.0; Debt-to-Equity Ratio: 5.514 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 20.0% -&gt; Score: 100; Profit CAGR 5Y: 25.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=48.71, MACD=Negative -&gt; Score: 24.677932862963523; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.54 -&gt; Penalty: 0.46; Final Rating: 27.07; Promoter Holding: 60.0% -&gt; Score: 100; Institutional Holding: 10.0% -&gt; Score: 40.0; Debt-to-Equity Ratio: 5.514 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 20.0% -&gt; Score: 100; Profit CAGR 5Y: 25.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=48.71, MACD=Negative -&gt; Score: 24.677932862963523; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.54 -&gt; Penalty: 0.46; Final Rating: 27.07; Promoter Holding: 60.0% -&gt; Score: 100; Institutional Holding: 10.0% -&gt; Score: 40.0; Debt-to-Equity Ratio: 5.514 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 20.0% -&gt; Score: 100; Profit CAGR 5Y: 25.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=48.71, MACD=Negative -&gt; Score: 24.677932862963523; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.54 -&gt; Penalty: 0.46; Final Rating: 27.07</t>
+          <t>Fetched fundamental data for CARTRADE.NS; Calculated technical metrics for CARTRADE.NS; Promoter Holding: 61.0% -&gt; Score: 100; Institutional Holding: 39.0% -&gt; Score: 100; Debt-to-Equity Ratio: 5.514 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 78.0% -&gt; Score: 100; Profit CAGR 5Y: 35.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=48.71, MACD=Negative -&gt; Score: 24.677932862963523; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.54 -&gt; Penalty: 0.46; Final Rating: 29.09; Promoter Holding: 61.0% -&gt; Score: 100; Institutional Holding: 39.0% -&gt; Score: 100; Debt-to-Equity Ratio: 5.514 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 78.0% -&gt; Score: 100; Profit CAGR 5Y: 35.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=48.71, MACD=Negative -&gt; Score: 24.677932862963523; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.54 -&gt; Penalty: 0.46; Final Rating: 29.09; Promoter Holding: 61.0% -&gt; Score: 100; Institutional Holding: 39.0% -&gt; Score: 100; Debt-to-Equity Ratio: 5.514 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 78.0% -&gt; Score: 100; Profit CAGR 5Y: 35.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=48.71, MACD=Negative -&gt; Score: 24.677932862963523; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.54 -&gt; Penalty: 0.46; Final Rating: 29.09; Promoter Holding: 61.0% -&gt; Score: 100; Institutional Holding: 39.0% -&gt; Score: 100; Debt-to-Equity Ratio: 5.514 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 78.0% -&gt; Score: 100; Profit CAGR 5Y: 35.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=48.71, MACD=Negative -&gt; Score: 24.677932862963523; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.54 -&gt; Penalty: 0.46; Final Rating: 29.09; Promoter Holding: 61.0% -&gt; Score: 100; Institutional Holding: 39.0% -&gt; Score: 100; Debt-to-Equity Ratio: 5.514 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 78.0% -&gt; Score: 100; Profit CAGR 5Y: 35.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=48.71, MACD=Negative -&gt; Score: 24.677932862963523; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.54 -&gt; Penalty: 0.46; Final Rating: 29.09; Promoter Holding: 61.0% -&gt; Score: 100; Institutional Holding: 39.0% -&gt; Score: 100; Debt-to-Equity Ratio: 5.514 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 78.0% -&gt; Score: 100; Profit CAGR 5Y: 35.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=48.71, MACD=Negative -&gt; Score: 24.677932862963523; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.54 -&gt; Penalty: 0.46; Final Rating: 29.09; Promoter Holding: 61.0% -&gt; Score: 100; Institutional Holding: 39.0% -&gt; Score: 100; Debt-to-Equity Ratio: 5.514 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 78.0% -&gt; Score: 100; Profit CAGR 5Y: 35.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=48.71, MACD=Negative -&gt; Score: 24.677932862963523; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.54 -&gt; Penalty: 0.46; Final Rating: 29.09; Promoter Holding: 61.0% -&gt; Score: 100; Institutional Holding: 39.0% -&gt; Score: 100; Debt-to-Equity Ratio: 5.514 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 78.0% -&gt; Score: 100; Profit CAGR 5Y: 35.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=48.71, MACD=Negative -&gt; Score: 24.677932862963523; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 100.00 -&gt; Score: 100; Volatility: 0.54 -&gt; Penalty: 0.46; Final Rating: 29.09</t>
         </is>
       </c>
     </row>
@@ -781,16 +781,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>34.24</v>
+        <v>40.53</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>50.0% -&gt; 100</t>
+          <t>49.93% -&gt; 99.86</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>15.0% -&gt; 60.0</t>
+          <t>42.0% -&gt; 100</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -805,12 +805,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>10.0% -&gt; 50.0</t>
+          <t>27.0% -&gt; 100</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>12.0% -&gt; 60.0</t>
+          <t>23.0% -&gt; 100</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -846,7 +846,7 @@
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>Fetched fundamental data for CHOLAFIN.NS; Calculated technical metrics for CHOLAFIN.NS; Promoter Holding: 50.0% -&gt; Score: 100; Institutional Holding: 15.0% -&gt; Score: 60.0; Debt-to-Equity Ratio: 738.948 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 10.0% -&gt; Score: 50.0; Profit CAGR 5Y: 12.0% -&gt; Score: 60.0; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=62.68, MACD=Positive -&gt; Score: 40.669056908105546; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 58.92 -&gt; Score: 58.915382323175486; Volatility: 0.35 -&gt; Penalty: 0.65; Final Rating: 34.24; Promoter Holding: 50.0% -&gt; Score: 100; Institutional Holding: 15.0% -&gt; Score: 60.0; Debt-to-Equity Ratio: 738.948 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 10.0% -&gt; Score: 50.0; Profit CAGR 5Y: 12.0% -&gt; Score: 60.0; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=62.68, MACD=Positive -&gt; Score: 40.669056908105546; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 58.92 -&gt; Score: 58.915382323175486; Volatility: 0.35 -&gt; Penalty: 0.65; Final Rating: 34.24; Promoter Holding: 50.0% -&gt; Score: 100; Institutional Holding: 15.0% -&gt; Score: 60.0; Debt-to-Equity Ratio: 738.948 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 10.0% -&gt; Score: 50.0; Profit CAGR 5Y: 12.0% -&gt; Score: 60.0; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=62.68, MACD=Positive -&gt; Score: 40.669056908105546; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 58.92 -&gt; Score: 58.915382323175486; Volatility: 0.35 -&gt; Penalty: 0.65; Final Rating: 34.24; Promoter Holding: 50.0% -&gt; Score: 100; Institutional Holding: 15.0% -&gt; Score: 60.0; Debt-to-Equity Ratio: 738.948 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 10.0% -&gt; Score: 50.0; Profit CAGR 5Y: 12.0% -&gt; Score: 60.0; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=62.68, MACD=Positive -&gt; Score: 40.669056908105546; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 58.92 -&gt; Score: 58.915382323175486; Volatility: 0.35 -&gt; Penalty: 0.65; Final Rating: 34.24; Promoter Holding: 50.0% -&gt; Score: 100; Institutional Holding: 15.0% -&gt; Score: 60.0; Debt-to-Equity Ratio: 738.948 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 10.0% -&gt; Score: 50.0; Profit CAGR 5Y: 12.0% -&gt; Score: 60.0; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=62.68, MACD=Positive -&gt; Score: 40.669056908105546; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 58.92 -&gt; Score: 58.915382323175486; Volatility: 0.35 -&gt; Penalty: 0.65; Final Rating: 34.24; Promoter Holding: 50.0% -&gt; Score: 100; Institutional Holding: 15.0% -&gt; Score: 60.0; Debt-to-Equity Ratio: 738.948 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 10.0% -&gt; Score: 50.0; Profit CAGR 5Y: 12.0% -&gt; Score: 60.0; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=62.68, MACD=Positive -&gt; Score: 40.669056908105546; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 58.92 -&gt; Score: 58.915382323175486; Volatility: 0.35 -&gt; Penalty: 0.65; Final Rating: 34.24; Promoter Holding: 50.0% -&gt; Score: 100; Institutional Holding: 15.0% -&gt; Score: 60.0; Debt-to-Equity Ratio: 738.948 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 10.0% -&gt; Score: 50.0; Profit CAGR 5Y: 12.0% -&gt; Score: 60.0; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=62.68, MACD=Positive -&gt; Score: 40.669056908105546; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 58.92 -&gt; Score: 58.915382323175486; Volatility: 0.35 -&gt; Penalty: 0.65; Final Rating: 34.24; Promoter Holding: 50.0% -&gt; Score: 100; Institutional Holding: 15.0% -&gt; Score: 60.0; Debt-to-Equity Ratio: 738.948 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 10.0% -&gt; Score: 50.0; Profit CAGR 5Y: 12.0% -&gt; Score: 60.0; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=62.68, MACD=Positive -&gt; Score: 40.669056908105546; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 58.92 -&gt; Score: 58.915382323175486; Volatility: 0.35 -&gt; Penalty: 0.65; Final Rating: 34.24</t>
+          <t>Fetched fundamental data for CHOLAFIN.NS; Calculated technical metrics for CHOLAFIN.NS; Promoter Holding: 49.93% -&gt; Score: 99.86; Institutional Holding: 42.0% -&gt; Score: 100; Debt-to-Equity Ratio: 738.948 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 27.0% -&gt; Score: 100; Profit CAGR 5Y: 23.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=62.68, MACD=Positive -&gt; Score: 40.669056908105546; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 58.92 -&gt; Score: 58.915382323175486; Volatility: 0.35 -&gt; Penalty: 0.65; Final Rating: 40.53; Promoter Holding: 49.93% -&gt; Score: 99.86; Institutional Holding: 42.0% -&gt; Score: 100; Debt-to-Equity Ratio: 738.948 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 27.0% -&gt; Score: 100; Profit CAGR 5Y: 23.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=62.68, MACD=Positive -&gt; Score: 40.669056908105546; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 58.92 -&gt; Score: 58.915382323175486; Volatility: 0.35 -&gt; Penalty: 0.65; Final Rating: 40.53; Promoter Holding: 49.93% -&gt; Score: 99.86; Institutional Holding: 42.0% -&gt; Score: 100; Debt-to-Equity Ratio: 738.948 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 27.0% -&gt; Score: 100; Profit CAGR 5Y: 23.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=62.68, MACD=Positive -&gt; Score: 40.669056908105546; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 58.92 -&gt; Score: 58.915382323175486; Volatility: 0.35 -&gt; Penalty: 0.65; Final Rating: 40.53; Promoter Holding: 49.93% -&gt; Score: 99.86; Institutional Holding: 42.0% -&gt; Score: 100; Debt-to-Equity Ratio: 738.948 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 27.0% -&gt; Score: 100; Profit CAGR 5Y: 23.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=62.68, MACD=Positive -&gt; Score: 40.669056908105546; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 58.92 -&gt; Score: 58.915382323175486; Volatility: 0.35 -&gt; Penalty: 0.65; Final Rating: 40.53; Promoter Holding: 49.93% -&gt; Score: 99.86; Institutional Holding: 42.0% -&gt; Score: 100; Debt-to-Equity Ratio: 738.948 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 27.0% -&gt; Score: 100; Profit CAGR 5Y: 23.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=62.68, MACD=Positive -&gt; Score: 40.669056908105546; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 58.92 -&gt; Score: 58.915382323175486; Volatility: 0.35 -&gt; Penalty: 0.65; Final Rating: 40.53; Promoter Holding: 49.93% -&gt; Score: 99.86; Institutional Holding: 42.0% -&gt; Score: 100; Debt-to-Equity Ratio: 738.948 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 27.0% -&gt; Score: 100; Profit CAGR 5Y: 23.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=62.68, MACD=Positive -&gt; Score: 40.669056908105546; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 58.92 -&gt; Score: 58.915382323175486; Volatility: 0.35 -&gt; Penalty: 0.65; Final Rating: 40.53; Promoter Holding: 49.93% -&gt; Score: 99.86; Institutional Holding: 42.0% -&gt; Score: 100; Debt-to-Equity Ratio: 738.948 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 27.0% -&gt; Score: 100; Profit CAGR 5Y: 23.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=62.68, MACD=Positive -&gt; Score: 40.669056908105546; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 58.92 -&gt; Score: 58.915382323175486; Volatility: 0.35 -&gt; Penalty: 0.65; Final Rating: 40.53; Promoter Holding: 49.93% -&gt; Score: 99.86; Institutional Holding: 42.0% -&gt; Score: 100; Debt-to-Equity Ratio: 738.948 -&gt; Score: 0; Return on Equity: 15.00% -&gt; Score: 75.0; Profit Growth YoY: 27.0% -&gt; Score: 100; Profit CAGR 5Y: 23.0% -&gt; Score: 100; Dividend Yield: 1.00% -&gt; Score: 50.0; Economic Moat: No moat: Insufficient competitive advantage -&gt; Score: 0; Valuation Score: PE=20.00, PB=2.00 -&gt; Score: 65.0; SymbolTrendRS: RSI=62.68, MACD=Positive -&gt; Score: 40.669056908105546; NIFTY200DMARSIVolume: Price &gt; 200-Day DMA (+25); NIFTY200DMARSIVolume: RSI in neutral range (+25); NIFTY200DMARSIVolume: Volume &lt;= 20-Day Vol MA (+10); NIFTY200DMARSIVolume: RS &gt; 50 (+25); NIFTY200DMARSIVolume: Total Score: 85; 200-Day DMA: Above -&gt; Score: 100; 14-Day RSI: Neutral -&gt; Score: 50; 20-Day Volume MA: Below -&gt; Score: 25; Simple RS vs ^NSEI: 58.92 -&gt; Score: 58.915382323175486; Volatility: 0.35 -&gt; Penalty: 0.65; Final Rating: 40.53</t>
         </is>
       </c>
     </row>
@@ -959,7 +959,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>NXPI: SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667649082</t>
+          <t>NXPI: SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667648925</t>
         </is>
       </c>
     </row>
@@ -1022,7 +1022,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>NXPI: Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.383570166515007</t>
+          <t>NXPI: Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.38357733960528</t>
         </is>
       </c>
     </row>
@@ -1106,7 +1106,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>NXPI: SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667649082</t>
+          <t>NXPI: SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667648925</t>
         </is>
       </c>
     </row>
@@ -1169,7 +1169,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>NXPI: Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.383570166515007</t>
+          <t>NXPI: Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.38357733960528</t>
         </is>
       </c>
     </row>
@@ -1253,7 +1253,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>NXPI: SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667649082</t>
+          <t>NXPI: SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667648925</t>
         </is>
       </c>
     </row>
@@ -1316,7 +1316,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>NXPI: Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.383570166515007</t>
+          <t>NXPI: Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.38357733960528</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>NXPI: SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667649082</t>
+          <t>NXPI: SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667648925</t>
         </is>
       </c>
     </row>
@@ -1463,7 +1463,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>NXPI: Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.383570166515007</t>
+          <t>NXPI: Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.38357733960528</t>
         </is>
       </c>
     </row>
@@ -1547,7 +1547,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>NXPI: SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667649082</t>
+          <t>NXPI: SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667648925</t>
         </is>
       </c>
     </row>
@@ -1610,7 +1610,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>NXPI: Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.383570166515007</t>
+          <t>NXPI: Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.38357733960528</t>
         </is>
       </c>
     </row>
@@ -1694,7 +1694,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>NXPI: SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667649082</t>
+          <t>NXPI: SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667648925</t>
         </is>
       </c>
     </row>
@@ -1757,7 +1757,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>NXPI: Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.383570166515007</t>
+          <t>NXPI: Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.38357733960528</t>
         </is>
       </c>
     </row>
@@ -1841,7 +1841,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>NXPI: SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667649082</t>
+          <t>NXPI: SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667648925</t>
         </is>
       </c>
     </row>
@@ -1904,7 +1904,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>NXPI: Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.383570166515007</t>
+          <t>NXPI: Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.38357733960528</t>
         </is>
       </c>
     </row>
@@ -1988,7 +1988,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>NXPI: SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667649082</t>
+          <t>NXPI: SymbolTrendRS: RSI=41.83, MACD=Positive -&gt; Score: 35.45860667648925</t>
         </is>
       </c>
     </row>
@@ -2051,7 +2051,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>NXPI: Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.383570166515007</t>
+          <t>NXPI: Simple RS vs ^IXIC: 30.38 -&gt; Score: 30.38357733960528</t>
         </is>
       </c>
     </row>
@@ -2086,14 +2086,14 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Promoter Holding: 50.6% -&gt; Score: 100</t>
+          <t>AXISCADES.NS: Promoter Holding: 59.4% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Institutional Holding: 8.7% -&gt; Score: 34.8</t>
+          <t>AXISCADES.NS: Institutional Holding: 3.0% -&gt; Score: 12.0</t>
         </is>
       </c>
     </row>
@@ -2114,14 +2114,14 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Profit Growth YoY: 38.5% -&gt; Score: 100</t>
+          <t>AXISCADES.NS: Profit Growth YoY: 34.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Profit CAGR 5Y: 11.5% -&gt; Score: 57.5</t>
+          <t>AXISCADES.NS: Profit CAGR 5Y: 85.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -2226,21 +2226,21 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Final Rating: 23.69</t>
+          <t>AXISCADES.NS: Final Rating: 24.3</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Promoter Holding: 50.6% -&gt; Score: 100</t>
+          <t>AXISCADES.NS: Promoter Holding: 59.4% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Institutional Holding: 8.7% -&gt; Score: 34.8</t>
+          <t>AXISCADES.NS: Institutional Holding: 3.0% -&gt; Score: 12.0</t>
         </is>
       </c>
     </row>
@@ -2261,14 +2261,14 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Profit Growth YoY: 38.5% -&gt; Score: 100</t>
+          <t>AXISCADES.NS: Profit Growth YoY: 34.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Profit CAGR 5Y: 11.5% -&gt; Score: 57.5</t>
+          <t>AXISCADES.NS: Profit CAGR 5Y: 85.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -2373,21 +2373,21 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Final Rating: 23.69</t>
+          <t>AXISCADES.NS: Final Rating: 24.3</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Promoter Holding: 50.6% -&gt; Score: 100</t>
+          <t>AXISCADES.NS: Promoter Holding: 59.4% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Institutional Holding: 8.7% -&gt; Score: 34.8</t>
+          <t>AXISCADES.NS: Institutional Holding: 3.0% -&gt; Score: 12.0</t>
         </is>
       </c>
     </row>
@@ -2408,14 +2408,14 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Profit Growth YoY: 38.5% -&gt; Score: 100</t>
+          <t>AXISCADES.NS: Profit Growth YoY: 34.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Profit CAGR 5Y: 11.5% -&gt; Score: 57.5</t>
+          <t>AXISCADES.NS: Profit CAGR 5Y: 85.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -2520,21 +2520,21 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Final Rating: 23.69</t>
+          <t>AXISCADES.NS: Final Rating: 24.3</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Promoter Holding: 50.6% -&gt; Score: 100</t>
+          <t>AXISCADES.NS: Promoter Holding: 59.4% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Institutional Holding: 8.7% -&gt; Score: 34.8</t>
+          <t>AXISCADES.NS: Institutional Holding: 3.0% -&gt; Score: 12.0</t>
         </is>
       </c>
     </row>
@@ -2555,14 +2555,14 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Profit Growth YoY: 38.5% -&gt; Score: 100</t>
+          <t>AXISCADES.NS: Profit Growth YoY: 34.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Profit CAGR 5Y: 11.5% -&gt; Score: 57.5</t>
+          <t>AXISCADES.NS: Profit CAGR 5Y: 85.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -2667,21 +2667,21 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Final Rating: 23.69</t>
+          <t>AXISCADES.NS: Final Rating: 24.3</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Promoter Holding: 50.6% -&gt; Score: 100</t>
+          <t>AXISCADES.NS: Promoter Holding: 59.4% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Institutional Holding: 8.7% -&gt; Score: 34.8</t>
+          <t>AXISCADES.NS: Institutional Holding: 3.0% -&gt; Score: 12.0</t>
         </is>
       </c>
     </row>
@@ -2702,14 +2702,14 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Profit Growth YoY: 38.5% -&gt; Score: 100</t>
+          <t>AXISCADES.NS: Profit Growth YoY: 34.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Profit CAGR 5Y: 11.5% -&gt; Score: 57.5</t>
+          <t>AXISCADES.NS: Profit CAGR 5Y: 85.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -2814,21 +2814,21 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Final Rating: 23.69</t>
+          <t>AXISCADES.NS: Final Rating: 24.3</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Promoter Holding: 50.6% -&gt; Score: 100</t>
+          <t>AXISCADES.NS: Promoter Holding: 59.4% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Institutional Holding: 8.7% -&gt; Score: 34.8</t>
+          <t>AXISCADES.NS: Institutional Holding: 3.0% -&gt; Score: 12.0</t>
         </is>
       </c>
     </row>
@@ -2849,14 +2849,14 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Profit Growth YoY: 38.5% -&gt; Score: 100</t>
+          <t>AXISCADES.NS: Profit Growth YoY: 34.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Profit CAGR 5Y: 11.5% -&gt; Score: 57.5</t>
+          <t>AXISCADES.NS: Profit CAGR 5Y: 85.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -2961,21 +2961,21 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Final Rating: 23.69</t>
+          <t>AXISCADES.NS: Final Rating: 24.3</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Promoter Holding: 50.6% -&gt; Score: 100</t>
+          <t>AXISCADES.NS: Promoter Holding: 59.4% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Institutional Holding: 8.7% -&gt; Score: 34.8</t>
+          <t>AXISCADES.NS: Institutional Holding: 3.0% -&gt; Score: 12.0</t>
         </is>
       </c>
     </row>
@@ -2996,14 +2996,14 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Profit Growth YoY: 38.5% -&gt; Score: 100</t>
+          <t>AXISCADES.NS: Profit Growth YoY: 34.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Profit CAGR 5Y: 11.5% -&gt; Score: 57.5</t>
+          <t>AXISCADES.NS: Profit CAGR 5Y: 85.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -3108,21 +3108,21 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Final Rating: 23.69</t>
+          <t>AXISCADES.NS: Final Rating: 24.3</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Promoter Holding: 50.6% -&gt; Score: 100</t>
+          <t>AXISCADES.NS: Promoter Holding: 59.4% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Institutional Holding: 8.7% -&gt; Score: 34.8</t>
+          <t>AXISCADES.NS: Institutional Holding: 3.0% -&gt; Score: 12.0</t>
         </is>
       </c>
     </row>
@@ -3143,14 +3143,14 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Profit Growth YoY: 38.5% -&gt; Score: 100</t>
+          <t>AXISCADES.NS: Profit Growth YoY: 34.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Profit CAGR 5Y: 11.5% -&gt; Score: 57.5</t>
+          <t>AXISCADES.NS: Profit CAGR 5Y: 85.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -3255,7 +3255,7 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>AXISCADES.NS: Final Rating: 23.69</t>
+          <t>AXISCADES.NS: Final Rating: 24.3</t>
         </is>
       </c>
     </row>
@@ -3276,14 +3276,14 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Promoter Holding: 60.0% -&gt; Score: 100</t>
+          <t>CARTRADE.NS: Promoter Holding: 61.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Institutional Holding: 10.0% -&gt; Score: 40.0</t>
+          <t>CARTRADE.NS: Institutional Holding: 39.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -3304,14 +3304,14 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Profit Growth YoY: 20.0% -&gt; Score: 100</t>
+          <t>CARTRADE.NS: Profit Growth YoY: 78.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Profit CAGR 5Y: 25.0% -&gt; Score: 100</t>
+          <t>CARTRADE.NS: Profit CAGR 5Y: 35.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -3416,21 +3416,21 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Final Rating: 27.07</t>
+          <t>CARTRADE.NS: Final Rating: 29.09</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Promoter Holding: 60.0% -&gt; Score: 100</t>
+          <t>CARTRADE.NS: Promoter Holding: 61.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Institutional Holding: 10.0% -&gt; Score: 40.0</t>
+          <t>CARTRADE.NS: Institutional Holding: 39.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -3451,14 +3451,14 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Profit Growth YoY: 20.0% -&gt; Score: 100</t>
+          <t>CARTRADE.NS: Profit Growth YoY: 78.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Profit CAGR 5Y: 25.0% -&gt; Score: 100</t>
+          <t>CARTRADE.NS: Profit CAGR 5Y: 35.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -3563,21 +3563,21 @@
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Final Rating: 27.07</t>
+          <t>CARTRADE.NS: Final Rating: 29.09</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Promoter Holding: 60.0% -&gt; Score: 100</t>
+          <t>CARTRADE.NS: Promoter Holding: 61.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Institutional Holding: 10.0% -&gt; Score: 40.0</t>
+          <t>CARTRADE.NS: Institutional Holding: 39.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -3598,14 +3598,14 @@
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Profit Growth YoY: 20.0% -&gt; Score: 100</t>
+          <t>CARTRADE.NS: Profit Growth YoY: 78.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Profit CAGR 5Y: 25.0% -&gt; Score: 100</t>
+          <t>CARTRADE.NS: Profit CAGR 5Y: 35.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -3710,21 +3710,21 @@
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Final Rating: 27.07</t>
+          <t>CARTRADE.NS: Final Rating: 29.09</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Promoter Holding: 60.0% -&gt; Score: 100</t>
+          <t>CARTRADE.NS: Promoter Holding: 61.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Institutional Holding: 10.0% -&gt; Score: 40.0</t>
+          <t>CARTRADE.NS: Institutional Holding: 39.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -3745,14 +3745,14 @@
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Profit Growth YoY: 20.0% -&gt; Score: 100</t>
+          <t>CARTRADE.NS: Profit Growth YoY: 78.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Profit CAGR 5Y: 25.0% -&gt; Score: 100</t>
+          <t>CARTRADE.NS: Profit CAGR 5Y: 35.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -3857,21 +3857,21 @@
     <row r="427">
       <c r="A427" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Final Rating: 27.07</t>
+          <t>CARTRADE.NS: Final Rating: 29.09</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Promoter Holding: 60.0% -&gt; Score: 100</t>
+          <t>CARTRADE.NS: Promoter Holding: 61.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Institutional Holding: 10.0% -&gt; Score: 40.0</t>
+          <t>CARTRADE.NS: Institutional Holding: 39.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -3892,14 +3892,14 @@
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Profit Growth YoY: 20.0% -&gt; Score: 100</t>
+          <t>CARTRADE.NS: Profit Growth YoY: 78.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Profit CAGR 5Y: 25.0% -&gt; Score: 100</t>
+          <t>CARTRADE.NS: Profit CAGR 5Y: 35.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -4004,21 +4004,21 @@
     <row r="448">
       <c r="A448" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Final Rating: 27.07</t>
+          <t>CARTRADE.NS: Final Rating: 29.09</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Promoter Holding: 60.0% -&gt; Score: 100</t>
+          <t>CARTRADE.NS: Promoter Holding: 61.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Institutional Holding: 10.0% -&gt; Score: 40.0</t>
+          <t>CARTRADE.NS: Institutional Holding: 39.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -4039,14 +4039,14 @@
     <row r="453">
       <c r="A453" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Profit Growth YoY: 20.0% -&gt; Score: 100</t>
+          <t>CARTRADE.NS: Profit Growth YoY: 78.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Profit CAGR 5Y: 25.0% -&gt; Score: 100</t>
+          <t>CARTRADE.NS: Profit CAGR 5Y: 35.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -4151,21 +4151,21 @@
     <row r="469">
       <c r="A469" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Final Rating: 27.07</t>
+          <t>CARTRADE.NS: Final Rating: 29.09</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Promoter Holding: 60.0% -&gt; Score: 100</t>
+          <t>CARTRADE.NS: Promoter Holding: 61.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Institutional Holding: 10.0% -&gt; Score: 40.0</t>
+          <t>CARTRADE.NS: Institutional Holding: 39.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -4186,14 +4186,14 @@
     <row r="474">
       <c r="A474" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Profit Growth YoY: 20.0% -&gt; Score: 100</t>
+          <t>CARTRADE.NS: Profit Growth YoY: 78.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Profit CAGR 5Y: 25.0% -&gt; Score: 100</t>
+          <t>CARTRADE.NS: Profit CAGR 5Y: 35.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -4298,21 +4298,21 @@
     <row r="490">
       <c r="A490" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Final Rating: 27.07</t>
+          <t>CARTRADE.NS: Final Rating: 29.09</t>
         </is>
       </c>
     </row>
     <row r="491">
       <c r="A491" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Promoter Holding: 60.0% -&gt; Score: 100</t>
+          <t>CARTRADE.NS: Promoter Holding: 61.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="492">
       <c r="A492" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Institutional Holding: 10.0% -&gt; Score: 40.0</t>
+          <t>CARTRADE.NS: Institutional Holding: 39.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -4333,14 +4333,14 @@
     <row r="495">
       <c r="A495" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Profit Growth YoY: 20.0% -&gt; Score: 100</t>
+          <t>CARTRADE.NS: Profit Growth YoY: 78.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="496">
       <c r="A496" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Profit CAGR 5Y: 25.0% -&gt; Score: 100</t>
+          <t>CARTRADE.NS: Profit CAGR 5Y: 35.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -4445,7 +4445,7 @@
     <row r="511">
       <c r="A511" t="inlineStr">
         <is>
-          <t>CARTRADE.NS: Final Rating: 27.07</t>
+          <t>CARTRADE.NS: Final Rating: 29.09</t>
         </is>
       </c>
     </row>
@@ -4466,14 +4466,14 @@
     <row r="514">
       <c r="A514" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Promoter Holding: 50.0% -&gt; Score: 100</t>
+          <t>CHOLAFIN.NS: Promoter Holding: 49.93% -&gt; Score: 99.86</t>
         </is>
       </c>
     </row>
     <row r="515">
       <c r="A515" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Institutional Holding: 15.0% -&gt; Score: 60.0</t>
+          <t>CHOLAFIN.NS: Institutional Holding: 42.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -4494,14 +4494,14 @@
     <row r="518">
       <c r="A518" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Profit Growth YoY: 10.0% -&gt; Score: 50.0</t>
+          <t>CHOLAFIN.NS: Profit Growth YoY: 27.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="519">
       <c r="A519" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Profit CAGR 5Y: 12.0% -&gt; Score: 60.0</t>
+          <t>CHOLAFIN.NS: Profit CAGR 5Y: 23.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -4606,21 +4606,21 @@
     <row r="534">
       <c r="A534" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Final Rating: 34.24</t>
+          <t>CHOLAFIN.NS: Final Rating: 40.53</t>
         </is>
       </c>
     </row>
     <row r="535">
       <c r="A535" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Promoter Holding: 50.0% -&gt; Score: 100</t>
+          <t>CHOLAFIN.NS: Promoter Holding: 49.93% -&gt; Score: 99.86</t>
         </is>
       </c>
     </row>
     <row r="536">
       <c r="A536" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Institutional Holding: 15.0% -&gt; Score: 60.0</t>
+          <t>CHOLAFIN.NS: Institutional Holding: 42.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -4641,14 +4641,14 @@
     <row r="539">
       <c r="A539" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Profit Growth YoY: 10.0% -&gt; Score: 50.0</t>
+          <t>CHOLAFIN.NS: Profit Growth YoY: 27.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="540">
       <c r="A540" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Profit CAGR 5Y: 12.0% -&gt; Score: 60.0</t>
+          <t>CHOLAFIN.NS: Profit CAGR 5Y: 23.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -4753,21 +4753,21 @@
     <row r="555">
       <c r="A555" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Final Rating: 34.24</t>
+          <t>CHOLAFIN.NS: Final Rating: 40.53</t>
         </is>
       </c>
     </row>
     <row r="556">
       <c r="A556" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Promoter Holding: 50.0% -&gt; Score: 100</t>
+          <t>CHOLAFIN.NS: Promoter Holding: 49.93% -&gt; Score: 99.86</t>
         </is>
       </c>
     </row>
     <row r="557">
       <c r="A557" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Institutional Holding: 15.0% -&gt; Score: 60.0</t>
+          <t>CHOLAFIN.NS: Institutional Holding: 42.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -4788,14 +4788,14 @@
     <row r="560">
       <c r="A560" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Profit Growth YoY: 10.0% -&gt; Score: 50.0</t>
+          <t>CHOLAFIN.NS: Profit Growth YoY: 27.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="561">
       <c r="A561" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Profit CAGR 5Y: 12.0% -&gt; Score: 60.0</t>
+          <t>CHOLAFIN.NS: Profit CAGR 5Y: 23.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -4900,21 +4900,21 @@
     <row r="576">
       <c r="A576" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Final Rating: 34.24</t>
+          <t>CHOLAFIN.NS: Final Rating: 40.53</t>
         </is>
       </c>
     </row>
     <row r="577">
       <c r="A577" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Promoter Holding: 50.0% -&gt; Score: 100</t>
+          <t>CHOLAFIN.NS: Promoter Holding: 49.93% -&gt; Score: 99.86</t>
         </is>
       </c>
     </row>
     <row r="578">
       <c r="A578" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Institutional Holding: 15.0% -&gt; Score: 60.0</t>
+          <t>CHOLAFIN.NS: Institutional Holding: 42.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -4935,14 +4935,14 @@
     <row r="581">
       <c r="A581" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Profit Growth YoY: 10.0% -&gt; Score: 50.0</t>
+          <t>CHOLAFIN.NS: Profit Growth YoY: 27.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="582">
       <c r="A582" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Profit CAGR 5Y: 12.0% -&gt; Score: 60.0</t>
+          <t>CHOLAFIN.NS: Profit CAGR 5Y: 23.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -5047,21 +5047,21 @@
     <row r="597">
       <c r="A597" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Final Rating: 34.24</t>
+          <t>CHOLAFIN.NS: Final Rating: 40.53</t>
         </is>
       </c>
     </row>
     <row r="598">
       <c r="A598" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Promoter Holding: 50.0% -&gt; Score: 100</t>
+          <t>CHOLAFIN.NS: Promoter Holding: 49.93% -&gt; Score: 99.86</t>
         </is>
       </c>
     </row>
     <row r="599">
       <c r="A599" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Institutional Holding: 15.0% -&gt; Score: 60.0</t>
+          <t>CHOLAFIN.NS: Institutional Holding: 42.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -5082,14 +5082,14 @@
     <row r="602">
       <c r="A602" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Profit Growth YoY: 10.0% -&gt; Score: 50.0</t>
+          <t>CHOLAFIN.NS: Profit Growth YoY: 27.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="603">
       <c r="A603" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Profit CAGR 5Y: 12.0% -&gt; Score: 60.0</t>
+          <t>CHOLAFIN.NS: Profit CAGR 5Y: 23.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -5194,21 +5194,21 @@
     <row r="618">
       <c r="A618" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Final Rating: 34.24</t>
+          <t>CHOLAFIN.NS: Final Rating: 40.53</t>
         </is>
       </c>
     </row>
     <row r="619">
       <c r="A619" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Promoter Holding: 50.0% -&gt; Score: 100</t>
+          <t>CHOLAFIN.NS: Promoter Holding: 49.93% -&gt; Score: 99.86</t>
         </is>
       </c>
     </row>
     <row r="620">
       <c r="A620" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Institutional Holding: 15.0% -&gt; Score: 60.0</t>
+          <t>CHOLAFIN.NS: Institutional Holding: 42.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -5229,14 +5229,14 @@
     <row r="623">
       <c r="A623" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Profit Growth YoY: 10.0% -&gt; Score: 50.0</t>
+          <t>CHOLAFIN.NS: Profit Growth YoY: 27.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="624">
       <c r="A624" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Profit CAGR 5Y: 12.0% -&gt; Score: 60.0</t>
+          <t>CHOLAFIN.NS: Profit CAGR 5Y: 23.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -5341,21 +5341,21 @@
     <row r="639">
       <c r="A639" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Final Rating: 34.24</t>
+          <t>CHOLAFIN.NS: Final Rating: 40.53</t>
         </is>
       </c>
     </row>
     <row r="640">
       <c r="A640" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Promoter Holding: 50.0% -&gt; Score: 100</t>
+          <t>CHOLAFIN.NS: Promoter Holding: 49.93% -&gt; Score: 99.86</t>
         </is>
       </c>
     </row>
     <row r="641">
       <c r="A641" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Institutional Holding: 15.0% -&gt; Score: 60.0</t>
+          <t>CHOLAFIN.NS: Institutional Holding: 42.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -5376,14 +5376,14 @@
     <row r="644">
       <c r="A644" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Profit Growth YoY: 10.0% -&gt; Score: 50.0</t>
+          <t>CHOLAFIN.NS: Profit Growth YoY: 27.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="645">
       <c r="A645" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Profit CAGR 5Y: 12.0% -&gt; Score: 60.0</t>
+          <t>CHOLAFIN.NS: Profit CAGR 5Y: 23.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -5488,21 +5488,21 @@
     <row r="660">
       <c r="A660" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Final Rating: 34.24</t>
+          <t>CHOLAFIN.NS: Final Rating: 40.53</t>
         </is>
       </c>
     </row>
     <row r="661">
       <c r="A661" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Promoter Holding: 50.0% -&gt; Score: 100</t>
+          <t>CHOLAFIN.NS: Promoter Holding: 49.93% -&gt; Score: 99.86</t>
         </is>
       </c>
     </row>
     <row r="662">
       <c r="A662" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Institutional Holding: 15.0% -&gt; Score: 60.0</t>
+          <t>CHOLAFIN.NS: Institutional Holding: 42.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -5523,14 +5523,14 @@
     <row r="665">
       <c r="A665" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Profit Growth YoY: 10.0% -&gt; Score: 50.0</t>
+          <t>CHOLAFIN.NS: Profit Growth YoY: 27.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
     <row r="666">
       <c r="A666" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Profit CAGR 5Y: 12.0% -&gt; Score: 60.0</t>
+          <t>CHOLAFIN.NS: Profit CAGR 5Y: 23.0% -&gt; Score: 100</t>
         </is>
       </c>
     </row>
@@ -5635,7 +5635,7 @@
     <row r="681">
       <c r="A681" t="inlineStr">
         <is>
-          <t>CHOLAFIN.NS: Final Rating: 34.24</t>
+          <t>CHOLAFIN.NS: Final Rating: 40.53</t>
         </is>
       </c>
     </row>

</xml_diff>